<commit_message>
updating puerto_rico_stoch for rivanna
</commit_message>
<xml_diff>
--- a/projects/puerto_rico_stoch/data/data_T.xlsx
+++ b/projects/puerto_rico_stoch/data/data_T.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FA027B-C788-4616-8B58-97A208DB0BF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460AC9D1-B50F-4321-8A4D-B8ABE5894EB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6861,7 +6861,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6923,7 +6923,7 @@
         <v>87</v>
       </c>
       <c r="D4" s="3">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -6937,7 +6937,7 @@
         <v>87</v>
       </c>
       <c r="D5">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated puerto rico stochastics post processing
</commit_message>
<xml_diff>
--- a/projects/puerto_rico_stoch/data/data_T.xlsx
+++ b/projects/puerto_rico_stoch/data/data_T.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C0938C-715B-4698-81EF-06F297C684F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A483A005-A0FE-488A-815D-71FE882321AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="941" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="220">
   <si>
     <t>connection</t>
   </si>
@@ -2141,8 +2141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2436,9 +2436,7 @@
       <c r="B12" s="6">
         <v>22</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>196</v>
-      </c>
+      <c r="C12" s="9"/>
       <c r="D12" s="6">
         <v>36.799999999999997</v>
       </c>
@@ -2459,11 +2457,9 @@
         <v>116</v>
       </c>
       <c r="B13" s="6">
-        <v>31</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>196</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C13" s="9"/>
       <c r="D13" s="6">
         <v>36.799999999999997</v>
       </c>
@@ -2659,9 +2655,7 @@
       <c r="B21" s="22">
         <v>22</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>196</v>
-      </c>
+      <c r="C21" s="22"/>
       <c r="D21" s="22">
         <v>36.799999999999997</v>
       </c>
@@ -2682,11 +2676,9 @@
         <v>122</v>
       </c>
       <c r="B22" s="22">
-        <v>31</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>196</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C22" s="22"/>
       <c r="D22" s="22">
         <v>36.799999999999997</v>
       </c>
@@ -2807,9 +2799,7 @@
       <c r="B27" s="6">
         <v>22</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>196</v>
-      </c>
+      <c r="C27" s="6"/>
       <c r="D27" s="6">
         <v>36.799999999999997</v>
       </c>
@@ -2830,11 +2820,9 @@
         <v>135</v>
       </c>
       <c r="B28" s="6">
-        <v>31</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>196</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C28" s="6"/>
       <c r="D28" s="6">
         <v>36.799999999999997</v>
       </c>
@@ -2861,7 +2849,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3296,7 +3284,7 @@
         <v>121</v>
       </c>
       <c r="B21" s="23">
-        <v>1130</v>
+        <v>1060</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="23">
@@ -6858,8 +6846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adjusted reserve margin constraint in temoa_stochastic updated model inputs
</commit_message>
<xml_diff>
--- a/projects/puerto_rico_stoch/data/data_T.xlsx
+++ b/projects/puerto_rico_stoch/data/data_T.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A483A005-A0FE-488A-815D-71FE882321AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F871D1-C925-4F49-BC9F-B04C6AF39095}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="941" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="222">
   <si>
     <t>connection</t>
   </si>
@@ -701,6 +701,12 @@
   </si>
   <si>
     <t>https://www.eia.gov/outlooks/aeo/assumptions/pdf/table_8.2.pdf, 2019</t>
+  </si>
+  <si>
+    <t>IRP</t>
+  </si>
+  <si>
+    <t>https://energia.pr.gov/en/integrated-resource-plan/</t>
   </si>
 </sst>
 </file>
@@ -1113,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,6 +1364,14 @@
       </c>
       <c r="C25" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -1373,6 +1387,7 @@
     <hyperlink ref="E21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="E23" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="E22" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E26" r:id="rId12" xr:uid="{A7FDCA60-4042-424F-BE01-B472EFA0655F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2141,8 +2156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2359,10 +2374,10 @@
         <v>112</v>
       </c>
       <c r="B9" s="9">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>136</v>
+        <v>220</v>
       </c>
       <c r="D9" s="9">
         <v>36.799999999999997</v>
@@ -2436,7 +2451,9 @@
       <c r="B12" s="6">
         <v>22</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="6" t="s">
+        <v>220</v>
+      </c>
       <c r="D12" s="6">
         <v>36.799999999999997</v>
       </c>
@@ -2459,7 +2476,9 @@
       <c r="B13" s="6">
         <v>25</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="6" t="s">
+        <v>220</v>
+      </c>
       <c r="D13" s="6">
         <v>36.799999999999997</v>
       </c>
@@ -2655,7 +2674,9 @@
       <c r="B21" s="22">
         <v>22</v>
       </c>
-      <c r="C21" s="22"/>
+      <c r="C21" s="22" t="s">
+        <v>220</v>
+      </c>
       <c r="D21" s="22">
         <v>36.799999999999997</v>
       </c>
@@ -2678,7 +2699,9 @@
       <c r="B22" s="22">
         <v>25</v>
       </c>
-      <c r="C22" s="22"/>
+      <c r="C22" s="22" t="s">
+        <v>220</v>
+      </c>
       <c r="D22" s="22">
         <v>36.799999999999997</v>
       </c>
@@ -2799,7 +2822,9 @@
       <c r="B27" s="6">
         <v>22</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>220</v>
+      </c>
       <c r="D27" s="6">
         <v>36.799999999999997</v>
       </c>
@@ -2822,7 +2847,9 @@
       <c r="B28" s="6">
         <v>25</v>
       </c>
-      <c r="C28" s="6"/>
+      <c r="C28" s="6" t="s">
+        <v>220</v>
+      </c>
       <c r="D28" s="6">
         <v>36.799999999999997</v>
       </c>
@@ -2848,8 +2875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3028,7 +3055,7 @@
         <v>112</v>
       </c>
       <c r="B9" s="6">
-        <v>3935</v>
+        <v>4022</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>196</v>
@@ -3053,7 +3080,7 @@
       <c r="B10" s="6"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12">
-        <v>425.4</v>
+        <v>425.38</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>142</v>
@@ -3150,7 +3177,7 @@
         <v>118</v>
       </c>
       <c r="B15" s="23">
-        <v>3749</v>
+        <v>3908</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>196</v>
@@ -3173,7 +3200,7 @@
         <v>215</v>
       </c>
       <c r="B16" s="23">
-        <v>3644</v>
+        <v>3981</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>196</v>
@@ -3196,17 +3223,17 @@
         <v>216</v>
       </c>
       <c r="B17" s="23">
-        <v>952</v>
+        <v>999</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="23">
+        <v>11.33</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" s="23">
         <v>1</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="F17" s="23">
-        <v>11.33</v>
       </c>
       <c r="G17" s="22" t="s">
         <v>195</v>
@@ -3217,17 +3244,17 @@
         <v>218</v>
       </c>
       <c r="B18" s="23">
-        <v>952</v>
+        <v>999</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="23">
+        <v>11.33</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="F18" s="23">
         <v>1</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="F18" s="23">
-        <v>11.33</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>195</v>
@@ -3284,9 +3311,11 @@
         <v>121</v>
       </c>
       <c r="B21" s="23">
-        <v>1060</v>
-      </c>
-      <c r="C21" s="22"/>
+        <v>1075</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>196</v>
+      </c>
       <c r="D21" s="23">
         <v>13</v>
       </c>
@@ -3305,7 +3334,7 @@
         <v>122</v>
       </c>
       <c r="B22" s="23">
-        <v>1494</v>
+        <v>1528</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>196</v>
@@ -3351,7 +3380,7 @@
         <v>132</v>
       </c>
       <c r="B24" s="7">
-        <v>3749</v>
+        <v>3908</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>196</v>
@@ -3420,9 +3449,11 @@
         <v>134</v>
       </c>
       <c r="B27" s="7">
-        <v>1460</v>
-      </c>
-      <c r="C27" s="6"/>
+        <v>1075</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="D27" s="7">
         <v>13</v>
       </c>
@@ -3441,7 +3472,7 @@
         <v>135</v>
       </c>
       <c r="B28" s="7">
-        <v>1494</v>
+        <v>1528</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>196</v>
@@ -3825,7 +3856,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4120,7 +4151,7 @@
         <v>112</v>
       </c>
       <c r="B21" s="13">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="C21" s="14">
         <v>1953</v>
@@ -4210,7 +4241,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4238,7 +4269,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0</v>
+        <v>0.26214999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -6844,19 +6875,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -6870,7 +6900,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -6884,7 +6914,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -6898,12 +6928,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2021</v>
       </c>
       <c r="B4" s="30">
-        <v>66.999600000000001</v>
+        <v>66.489999999999995</v>
       </c>
       <c r="C4" t="s">
         <v>87</v>
@@ -6912,12 +6942,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2026</v>
       </c>
       <c r="B5" s="30">
-        <v>66.103200000000001</v>
+        <v>67.28</v>
       </c>
       <c r="C5" t="s">
         <v>87</v>
@@ -6925,14 +6955,13 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="29"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2031</v>
       </c>
       <c r="B6" s="30">
-        <v>65.77</v>
+        <v>65.319999999999993</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>87</v>
@@ -6940,14 +6969,13 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="29"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2036</v>
       </c>
       <c r="B7" s="30">
-        <v>65.47</v>
+        <v>63.75</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>87</v>
@@ -6955,22 +6983,20 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="29"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2041</v>
       </c>
       <c r="B8" s="30">
-        <v>65.41</v>
+        <v>63.75</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="29">
         <v>0</v>
       </c>
-      <c r="E8" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7026,7 +7052,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7173,6 +7199,9 @@
       </c>
       <c r="K4" t="s">
         <v>184</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2028</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
running with reserve margin and updated energy storage constraints
</commit_message>
<xml_diff>
--- a/projects/puerto_rico_stoch/data/data_T.xlsx
+++ b/projects/puerto_rico_stoch/data/data_T.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F871D1-C925-4F49-BC9F-B04C6AF39095}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE78AB0D-7B8A-4F22-9F90-E20B838C63A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="941" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -4281,7 +4281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
@@ -6877,7 +6877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated version reserve margin with capacity credit
</commit_message>
<xml_diff>
--- a/projects/puerto_rico_stoch/data/data_T.xlsx
+++ b/projects/puerto_rico_stoch/data/data_T.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE78AB0D-7B8A-4F22-9F90-E20B838C63A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB379211-5C84-41AD-9F25-56175B05BA2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="941" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -16,8 +16,8 @@
     <sheet name="Demand" sheetId="3" r:id="rId6"/>
     <sheet name="DiscountRate" sheetId="5" r:id="rId7"/>
     <sheet name="Fuels" sheetId="6" r:id="rId8"/>
-    <sheet name="FuelsExisting" sheetId="7" r:id="rId9"/>
-    <sheet name="PowerPlants" sheetId="8" r:id="rId10"/>
+    <sheet name="PowerPlants" sheetId="8" r:id="rId9"/>
+    <sheet name="FuelsExisting" sheetId="7" r:id="rId10"/>
     <sheet name="PowerPlantsPerformance" sheetId="12" r:id="rId11"/>
     <sheet name="PowerPlantsCosts" sheetId="10" r:id="rId12"/>
     <sheet name="PowerPlantsConstraints" sheetId="9" r:id="rId13"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="224">
   <si>
     <t>connection</t>
   </si>
@@ -707,6 +707,12 @@
   </si>
   <si>
     <t>https://energia.pr.gov/en/integrated-resource-plan/</t>
+  </si>
+  <si>
+    <t>CapacityCredit</t>
+  </si>
+  <si>
+    <t>[fr]</t>
   </si>
 </sst>
 </file>
@@ -828,7 +834,21 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1394,761 +1414,59 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G14" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G15" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H20" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G21" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="H21" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G22" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>129</v>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1920</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2015</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:H15 D19:H28">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16:H18">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4281,7 +3599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
@@ -6877,8 +6195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7363,58 +6681,854 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1920</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2015</v>
+      <c r="C2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I5">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I8">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I12">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I13">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="I14">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I15">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I18">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I19">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I20">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I21">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="I23">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I26">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I27">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28">
+        <v>0.36</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D3:D15 D19:D28 F19:H28 F3:H15">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D18 F16:H18">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E15 E19:E28">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:E18">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>